<commit_message>
fixed ASC sub2 excel structure
</commit_message>
<xml_diff>
--- a/ccbhc_measurements/dashboard/excel files/ASC_sub_2.xlsx
+++ b/ccbhc_measurements/dashboard/excel files/ASC_sub_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>numerator_time</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>medicaid</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -474,6 +479,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,6 +502,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -514,6 +525,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -534,6 +548,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +571,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -574,6 +594,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -594,6 +617,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -614,6 +640,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -634,6 +663,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -654,6 +686,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -674,6 +709,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -694,6 +732,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -714,6 +755,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -734,6 +778,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E15" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -754,6 +801,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -774,6 +824,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -794,6 +847,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -814,6 +870,9 @@
           <t>Counseling happened within a month</t>
         </is>
       </c>
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -834,6 +893,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -854,6 +916,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -874,6 +939,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E22" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -894,6 +962,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -914,6 +985,9 @@
           <t>Counseling happened immediately</t>
         </is>
       </c>
+      <c r="E24" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -934,6 +1008,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -954,6 +1031,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -974,6 +1054,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -994,6 +1077,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1014,6 +1100,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1034,6 +1123,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1054,6 +1146,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1074,6 +1169,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1094,6 +1192,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E33" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1114,6 +1215,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1134,6 +1238,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1154,6 +1261,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1174,6 +1284,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1194,6 +1307,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1214,6 +1330,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1234,6 +1353,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1254,6 +1376,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1274,6 +1399,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1294,6 +1422,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1314,6 +1445,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1334,6 +1468,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1354,6 +1491,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1374,6 +1514,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1394,6 +1537,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1414,6 +1560,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1434,6 +1583,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1454,6 +1606,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1474,6 +1629,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1494,6 +1652,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1514,6 +1675,9 @@
           <t>Counseling happened within a month</t>
         </is>
       </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1534,6 +1698,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1554,6 +1721,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1574,6 +1744,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1594,6 +1767,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1614,6 +1790,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1634,6 +1813,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1654,6 +1836,9 @@
           <t>Counseling happened within a week</t>
         </is>
       </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1674,6 +1859,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E62" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1694,6 +1882,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1714,6 +1905,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1734,6 +1928,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1754,6 +1951,9 @@
           <t>Counseling did not happen</t>
         </is>
       </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1773,6 +1973,9 @@
         <is>
           <t>Counseling happened immediately</t>
         </is>
+      </c>
+      <c r="E67" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ASC excel files
</commit_message>
<xml_diff>
--- a/ccbhc_measurements/dashboard/excel files/ASC_sub_2.xlsx
+++ b/ccbhc_measurements/dashboard/excel files/ASC_sub_2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,15 +446,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>counseling_id</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>numerator</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>numerator_time</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>numerator_desc</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>medicaid</t>
         </is>
@@ -471,15 +476,16 @@
           <t>10874-2024</t>
         </is>
       </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E2" t="b">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -494,15 +500,16 @@
           <t>11710-2024</t>
         </is>
       </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E3" t="b">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F3" t="b">
         <v>0</v>
       </c>
     </row>
@@ -517,15 +524,16 @@
           <t>11815-2024</t>
         </is>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E4" t="b">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -540,15 +548,16 @@
           <t>12947-2024</t>
         </is>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E5" t="b">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F5" t="b">
         <v>0</v>
       </c>
     </row>
@@ -563,15 +572,16 @@
           <t>15772-2024</t>
         </is>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -586,15 +596,16 @@
           <t>16464-2024</t>
         </is>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E7" t="b">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F7" t="b">
         <v>0</v>
       </c>
     </row>
@@ -609,15 +620,16 @@
           <t>18906-2024</t>
         </is>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E8" t="b">
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F8" t="b">
         <v>0</v>
       </c>
     </row>
@@ -632,15 +644,16 @@
           <t>20729-2024</t>
         </is>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E9" t="b">
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F9" t="b">
         <v>0</v>
       </c>
     </row>
@@ -655,15 +668,16 @@
           <t>22085-2024</t>
         </is>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E10" t="b">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F10" t="b">
         <v>0</v>
       </c>
     </row>
@@ -678,15 +692,16 @@
           <t>22381-2024</t>
         </is>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E11" t="b">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F11" t="b">
         <v>0</v>
       </c>
     </row>
@@ -701,15 +716,16 @@
           <t>25628-2024</t>
         </is>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E12" t="b">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F12" t="b">
         <v>0</v>
       </c>
     </row>
@@ -724,15 +740,16 @@
           <t>26404-2024</t>
         </is>
       </c>
-      <c r="C13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E13" t="b">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -747,15 +764,16 @@
           <t>26431-2024</t>
         </is>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E14" t="b">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F14" t="b">
         <v>0</v>
       </c>
     </row>
@@ -770,15 +788,16 @@
           <t>26830-2024</t>
         </is>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E15" t="b">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F15" t="b">
         <v>0</v>
       </c>
     </row>
@@ -793,15 +812,16 @@
           <t>26865-2024</t>
         </is>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E16" t="b">
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F16" t="b">
         <v>0</v>
       </c>
     </row>
@@ -816,15 +836,16 @@
           <t>27698-2024</t>
         </is>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E17" t="b">
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F17" t="b">
         <v>0</v>
       </c>
     </row>
@@ -839,15 +860,16 @@
           <t>27870-2024</t>
         </is>
       </c>
-      <c r="C18" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E18" t="b">
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -862,15 +884,20 @@
           <t>28868-2024</t>
         </is>
       </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="inlineStr">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>40716</t>
+        </is>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>Counseling happened within a month</t>
         </is>
       </c>
-      <c r="E19" t="b">
+      <c r="F19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -885,15 +912,16 @@
           <t>29933-2024</t>
         </is>
       </c>
-      <c r="C20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E20" t="b">
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F20" t="b">
         <v>0</v>
       </c>
     </row>
@@ -908,15 +936,16 @@
           <t>30469-2024</t>
         </is>
       </c>
-      <c r="C21" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E21" t="b">
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F21" t="b">
         <v>0</v>
       </c>
     </row>
@@ -931,15 +960,16 @@
           <t>30759-2024</t>
         </is>
       </c>
-      <c r="C22" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E22" t="b">
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F22" t="b">
         <v>0</v>
       </c>
     </row>
@@ -954,15 +984,16 @@
           <t>31332-2024</t>
         </is>
       </c>
-      <c r="C23" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E23" t="b">
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F23" t="b">
         <v>0</v>
       </c>
     </row>
@@ -977,15 +1008,20 @@
           <t>32985-2024</t>
         </is>
       </c>
-      <c r="C24" t="b">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>39325</t>
+        </is>
+      </c>
+      <c r="D24" t="b">
         <v>1</v>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>Counseling happened immediately</t>
         </is>
       </c>
-      <c r="E24" t="b">
+      <c r="F24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1000,15 +1036,16 @@
           <t>34867-2024</t>
         </is>
       </c>
-      <c r="C25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E25" t="b">
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F25" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1023,15 +1060,16 @@
           <t>36462-2024</t>
         </is>
       </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E26" t="b">
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F26" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1046,15 +1084,16 @@
           <t>36539-2024</t>
         </is>
       </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E27" t="b">
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1069,15 +1108,16 @@
           <t>38678-2024</t>
         </is>
       </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E28" t="b">
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F28" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1092,15 +1132,20 @@
           <t>39150-2024</t>
         </is>
       </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E29" t="b">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>56423</t>
+        </is>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Counseling happened within two months</t>
+        </is>
+      </c>
+      <c r="F29" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1115,15 +1160,16 @@
           <t>40205-2024</t>
         </is>
       </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E30" t="b">
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1138,15 +1184,16 @@
           <t>40230-2024</t>
         </is>
       </c>
-      <c r="C31" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E31" t="b">
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F31" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1161,15 +1208,20 @@
           <t>40571-2024</t>
         </is>
       </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E32" t="b">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>45311</t>
+        </is>
+      </c>
+      <c r="D32" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Counseling happened within two months</t>
+        </is>
+      </c>
+      <c r="F32" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1184,15 +1236,16 @@
           <t>43577-2024</t>
         </is>
       </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E33" t="b">
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F33" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1207,15 +1260,16 @@
           <t>44221-2024</t>
         </is>
       </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E34" t="b">
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F34" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1230,15 +1284,16 @@
           <t>45147-2024</t>
         </is>
       </c>
-      <c r="C35" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E35" t="b">
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F35" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1253,15 +1308,16 @@
           <t>51356-2024</t>
         </is>
       </c>
-      <c r="C36" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E36" t="b">
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F36" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1276,15 +1332,16 @@
           <t>51857-2024</t>
         </is>
       </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E37" t="b">
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F37" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1299,15 +1356,16 @@
           <t>52392-2024</t>
         </is>
       </c>
-      <c r="C38" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E38" t="b">
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F38" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1322,15 +1380,16 @@
           <t>52435-2024</t>
         </is>
       </c>
-      <c r="C39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E39" t="b">
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F39" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1345,15 +1404,16 @@
           <t>52593-2024</t>
         </is>
       </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E40" t="b">
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1368,15 +1428,16 @@
           <t>52698-2024</t>
         </is>
       </c>
-      <c r="C41" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E41" t="b">
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F41" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1391,15 +1452,16 @@
           <t>52959-2024</t>
         </is>
       </c>
-      <c r="C42" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E42" t="b">
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F42" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1414,15 +1476,16 @@
           <t>53291-2024</t>
         </is>
       </c>
-      <c r="C43" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E43" t="b">
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F43" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1437,15 +1500,16 @@
           <t>53314-2024</t>
         </is>
       </c>
-      <c r="C44" t="b">
-        <v>0</v>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E44" t="b">
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F44" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1460,15 +1524,16 @@
           <t>55069-2024</t>
         </is>
       </c>
-      <c r="C45" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E45" t="b">
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F45" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1483,15 +1548,16 @@
           <t>55761-2024</t>
         </is>
       </c>
-      <c r="C46" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E46" t="b">
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F46" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1506,15 +1572,16 @@
           <t>56719-2024</t>
         </is>
       </c>
-      <c r="C47" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E47" t="b">
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F47" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1529,15 +1596,16 @@
           <t>57439-2024</t>
         </is>
       </c>
-      <c r="C48" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E48" t="b">
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F48" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1552,15 +1620,16 @@
           <t>58765-2024</t>
         </is>
       </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E49" t="b">
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F49" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1575,15 +1644,16 @@
           <t>59770-2024</t>
         </is>
       </c>
-      <c r="C50" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E50" t="b">
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F50" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1598,15 +1668,16 @@
           <t>61096-2024</t>
         </is>
       </c>
-      <c r="C51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E51" t="b">
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F51" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1621,15 +1692,16 @@
           <t>61341-2024</t>
         </is>
       </c>
-      <c r="C52" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E52" t="b">
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F52" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1644,15 +1716,16 @@
           <t>64607-2024</t>
         </is>
       </c>
-      <c r="C53" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E53" t="b">
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F53" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1667,15 +1740,20 @@
           <t>65490-2024</t>
         </is>
       </c>
-      <c r="C54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" t="inlineStr">
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>65226</t>
+        </is>
+      </c>
+      <c r="D54" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" t="inlineStr">
         <is>
           <t>Counseling happened within a month</t>
         </is>
       </c>
-      <c r="E54" t="b">
+      <c r="F54" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1690,15 +1768,16 @@
           <t>68341-2024</t>
         </is>
       </c>
-      <c r="C55" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E55" t="b">
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F55" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1713,15 +1792,16 @@
           <t>69696-2024</t>
         </is>
       </c>
-      <c r="C56" t="b">
-        <v>0</v>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E56" t="b">
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1736,15 +1816,16 @@
           <t>70518-2024</t>
         </is>
       </c>
-      <c r="C57" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E57" t="b">
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F57" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1759,15 +1840,16 @@
           <t>77722-2024</t>
         </is>
       </c>
-      <c r="C58" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E58" t="b">
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1782,15 +1864,16 @@
           <t>78106-2024</t>
         </is>
       </c>
-      <c r="C59" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E59" t="b">
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F59" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1805,15 +1888,16 @@
           <t>78838-2024</t>
         </is>
       </c>
-      <c r="C60" t="b">
-        <v>0</v>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E60" t="b">
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F60" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1828,15 +1912,20 @@
           <t>80805-2024</t>
         </is>
       </c>
-      <c r="C61" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" t="inlineStr">
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>92447</t>
+        </is>
+      </c>
+      <c r="D61" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" t="inlineStr">
         <is>
           <t>Counseling happened within a week</t>
         </is>
       </c>
-      <c r="E61" t="b">
+      <c r="F61" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1851,15 +1940,16 @@
           <t>87150-2024</t>
         </is>
       </c>
-      <c r="C62" t="b">
-        <v>0</v>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E62" t="b">
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F62" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1874,15 +1964,16 @@
           <t>90852-2024</t>
         </is>
       </c>
-      <c r="C63" t="b">
-        <v>0</v>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E63" t="b">
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F63" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1897,15 +1988,16 @@
           <t>95946-2024</t>
         </is>
       </c>
-      <c r="C64" t="b">
-        <v>0</v>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E64" t="b">
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="b">
+        <v>0</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F64" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1920,15 +2012,16 @@
           <t>97948-2024</t>
         </is>
       </c>
-      <c r="C65" t="b">
-        <v>0</v>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E65" t="b">
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F65" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1943,15 +2036,16 @@
           <t>99902-2024</t>
         </is>
       </c>
-      <c r="C66" t="b">
-        <v>0</v>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Counseling did not happen</t>
-        </is>
-      </c>
-      <c r="E66" t="b">
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="b">
+        <v>0</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Counseling did not happen</t>
+        </is>
+      </c>
+      <c r="F66" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1966,15 +2060,20 @@
           <t>99932-2024</t>
         </is>
       </c>
-      <c r="C67" t="b">
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>23497</t>
+        </is>
+      </c>
+      <c r="D67" t="b">
         <v>1</v>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>Counseling happened immediately</t>
         </is>
       </c>
-      <c r="E67" t="b">
+      <c r="F67" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>